<commit_message>
use APIVIEW and ModelViewset
</commit_message>
<xml_diff>
--- a/media/product_sales_summary.xlsx
+++ b/media/product_sales_summary.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nike</t>
   </si>
   <si>
-    <t>men_cloths</t>
-  </si>
-  <si>
     <t>Footwear</t>
-  </si>
-  <si>
-    <t>cloths</t>
   </si>
   <si>
     <t>Product Name</t>
@@ -381,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,19 +383,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -409,33 +403,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
       <c r="E2">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>1200</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>